<commit_message>
0223 farmerManagement organize and add farmerso
</commit_message>
<xml_diff>
--- a/DataTable/FarmerTable.xlsx
+++ b/DataTable/FarmerTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seh00n/GitHub/ProjectF/DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\ProjectF\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDEAD60-B32D-044D-B62C-57544F179354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D3C26F-2EE2-4B83-9D53-37F73C20038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="-18460" windowWidth="28300" windowHeight="17440" xr2:uid="{7EF9CFC2-BCD5-964D-8D33-B289F6ACD1DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7EF9CFC2-BCD5-964D-8D33-B289F6ACD1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="FarmerTable" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -66,13 +66,25 @@
   </si>
   <si>
     <t>farmer_name_0</t>
+  </si>
+  <si>
+    <t>rarity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Erarity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -543,40 +555,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D7D4E3-B342-DD44-8AF7-A000D70DEC11}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19" thickBot="1"/>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="19" thickBot="1">
+    <row r="3" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="19" thickBot="1">
+    <row r="4" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0317 Sales Multiplier define to datatable
</commit_message>
<xml_diff>
--- a/DataTable/FarmerTable.xlsx
+++ b/DataTable/FarmerTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\ProjectF\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D3C26F-2EE2-4B83-9D53-37F73C20038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D511CE3-41A0-46FC-8703-B3F795D2BCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7EF9CFC2-BCD5-964D-8D33-B289F6ACD1DC}"/>
   </bookViews>
@@ -72,11 +72,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Erarity</t>
+    <t>Common</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Common</t>
+    <t>ERarity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -558,7 +558,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -585,7 +585,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -596,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>

</xml_diff>